<commit_message>
Added new lora, added rgb leds, updated TSP65988 schematic, added bat to 3v3, added battery balancer
</commit_message>
<xml_diff>
--- a/components.xlsx
+++ b/components.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Tartu Ülikool - arvutitehnika\Riistvara projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jako\Riistvara-projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>E-ink</t>
   </si>
@@ -32,9 +32,6 @@
     <t>link</t>
   </si>
   <si>
-    <t>doc</t>
-  </si>
-  <si>
     <t>hind</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>https://www.mouser.ee/ProductDetail/Espressif-Systems/ESP32-S3-WROOM-1-N16R8?qs=sGAEpiMZZMu3sxpa5v1qrkR%2F6t0IkXq81YLrKdmkb4Q%3D</t>
   </si>
   <si>
-    <t>LoRa</t>
-  </si>
-  <si>
     <t>LoRa antenn</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>https://www.elfadistrelec.ee/et/pijuice-lipo-battery-12000mah-pi-supply-pis-1129/p/30163381</t>
   </si>
   <si>
-    <t>USB PD</t>
-  </si>
-  <si>
     <t>https://www.mouser.ee/ProductDetail/Texas-Instruments/BQ25731RSNR?qs=stqOd1AaK7%2Fv1jry38xYIQ%3D%3D</t>
   </si>
   <si>
@@ -101,22 +92,58 @@
     <t>Speaker amplifier</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/4000076778363.html</t>
-  </si>
-  <si>
     <t>https://www.aliexpress.com/item/1005004214252441.html</t>
   </si>
   <si>
-    <t>Levelshifter/isolator</t>
-  </si>
-  <si>
-    <t>IO connectors</t>
-  </si>
-  <si>
     <t>https://www.mouser.ee/ProductDetail/Texas-Instruments/TPS65988DJRSHR?qs=T3oQrply3y8cml9f5FMm3A%3D%3D</t>
   </si>
   <si>
     <t>https://eu.mouser.com/ProductDetail/Hirose-Connector/CX90MWD2G-24P?qs=bAKSY%2FctAC6h%2FxOP2g12BQ%3D%3D</t>
+  </si>
+  <si>
+    <t>USB-PD battery</t>
+  </si>
+  <si>
+    <t>USB-PD negotiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB - UART </t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Silicon-Labs/CP2102N-A02-GQFN20?qs=u16ybLDytRaG8WdlP0fT2g%3D%3D</t>
+  </si>
+  <si>
+    <t>Digi pote</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Microchip-Technology-Atmel/MCP40D18T-503E-LT?qs=dQMF8gqycOVbxabKF9CRwQ%3D%3D</t>
+  </si>
+  <si>
+    <t>Bat to USB-c</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Monolithic-Power-Systems-MPS/MP2229GQ-P?qs=ZNK0BnemlqHKDD1LC56W1w%3D%3D</t>
+  </si>
+  <si>
+    <t>kogus</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005002702535557.html</t>
+  </si>
+  <si>
+    <t>LoRa Ra-01SH</t>
+  </si>
+  <si>
+    <t>Bat balancer</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Texas-Instruments/BQ29209DRBR?qs=hEBn5lgDlCoqdeLwAzko8w%3D%3D</t>
+  </si>
+  <si>
+    <t>RGB LED</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32453497583.html</t>
   </si>
 </sst>
 </file>
@@ -166,8 +193,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hüperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normaallaad" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -183,7 +210,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office'i kujundus">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -445,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,163 +489,380 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1">
-        <f>SUM(C:C)</f>
-        <v>81.090000000000018</v>
+        <f>SUM(E:E)</f>
+        <v>60.620000000000012</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>1.43</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2*D2</f>
+        <v>1.43</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>14.15</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E28" si="0">C3*D3</f>
+        <v>14.15</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>1.89</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>1.89</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>10.98</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>10.98</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
       <c r="C6">
         <v>4.3099999999999996</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>4.3099999999999996</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C7">
-        <v>3.21</v>
+        <v>5.42</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>5.42</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>1.24</v>
       </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1.24</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>36.909999999999997</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>3.79</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>3.79</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11">
-        <v>2.59</v>
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>0.59</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.59</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>2.16</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>6.64</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21">
+        <v>0.69</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22">
+        <v>2.84</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23">
+        <v>0.96</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added digi-pote symbol, added USB_source voltage regulators
</commit_message>
<xml_diff>
--- a/components.xlsx
+++ b/components.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>E-ink</t>
   </si>
@@ -98,9 +98,6 @@
     <t>https://www.mouser.ee/ProductDetail/Texas-Instruments/TPS65988DJRSHR?qs=T3oQrply3y8cml9f5FMm3A%3D%3D</t>
   </si>
   <si>
-    <t>https://eu.mouser.com/ProductDetail/Hirose-Connector/CX90MWD2G-24P?qs=bAKSY%2FctAC6h%2FxOP2g12BQ%3D%3D</t>
-  </si>
-  <si>
     <t>USB-PD battery</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>Digi pote</t>
   </si>
   <si>
-    <t>https://www.mouser.ee/ProductDetail/Microchip-Technology-Atmel/MCP40D18T-503E-LT?qs=dQMF8gqycOVbxabKF9CRwQ%3D%3D</t>
-  </si>
-  <si>
     <t>Bat to USB-c</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
     <t>kogus</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/1005002702535557.html</t>
-  </si>
-  <si>
     <t>LoRa Ra-01SH</t>
   </si>
   <si>
@@ -144,6 +135,24 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/32453497583.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/4001148156263.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005003210911840.html</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/TE-Connectivity/2305018-2?qs=EU6FO9ffTwfL23TDwkN0SQ%3D%3D</t>
+  </si>
+  <si>
+    <t>Proximity card</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/33016782798.html</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Microchip-Technology-Atmel/MCP4019T-502E-LT?qs=%2FsslhGPpiOTvaIZO0TEW6Q%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -472,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +493,7 @@
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -492,17 +501,17 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1">
         <f>SUM(E:E)</f>
-        <v>60.620000000000012</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>66.303200000000004</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -520,7 +529,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -538,7 +547,7 @@
         <v>14.15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -556,7 +565,7 @@
         <v>1.89</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -574,7 +583,7 @@
         <v>10.98</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -592,25 +601,25 @@
         <v>4.3099999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C7">
-        <v>5.42</v>
+        <v>4.82</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>5.42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4.82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -628,7 +637,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -646,9 +655,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -664,22 +673,28 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
+      </c>
+      <c r="C11">
+        <v>2.5499999999999998</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -688,7 +703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -697,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -715,19 +730,26 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="C15">
+        <f>9.86/100</f>
+        <v>9.8599999999999993E-2</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.1831999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -741,10 +763,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
         <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
       </c>
       <c r="C18">
         <v>2.16</v>
@@ -759,7 +781,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
@@ -783,10 +805,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C21">
         <v>0.69</v>
@@ -801,10 +823,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C22">
         <v>2.84</v>
@@ -819,10 +841,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C23">
         <v>0.96</v>
@@ -842,6 +864,12 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
       <c r="E25">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
added audio ref schematic, added bat to 5V, added shift register, connected devices with other periferals
</commit_message>
<xml_diff>
--- a/components.xlsx
+++ b/components.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jako\Riistvara-projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Tartu Ülikool - arvutitehnika\Riistvara projekt\airsoft_controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>E-ink</t>
   </si>
@@ -62,12 +62,6 @@
     <t>https://www.mouser.ee/ProductDetail/Linx-Technologies/ANT-868-HESM?qs=hWgE7mdIu5TTyqPbNERfhg%3D%3D</t>
   </si>
   <si>
-    <t>aku</t>
-  </si>
-  <si>
-    <t>https://www.elfadistrelec.ee/et/pijuice-lipo-battery-12000mah-pi-supply-pis-1129/p/30163381</t>
-  </si>
-  <si>
     <t>https://www.mouser.ee/ProductDetail/Texas-Instruments/BQ25731RSNR?qs=stqOd1AaK7%2Fv1jry38xYIQ%3D%3D</t>
   </si>
   <si>
@@ -83,15 +77,9 @@
     <t>USB-C</t>
   </si>
   <si>
-    <t>Piezo speaker</t>
-  </si>
-  <si>
     <t>SD card holder</t>
   </si>
   <si>
-    <t>Speaker amplifier</t>
-  </si>
-  <si>
     <t>https://www.aliexpress.com/item/1005004214252441.html</t>
   </si>
   <si>
@@ -110,9 +98,6 @@
     <t>https://www.mouser.ee/ProductDetail/Silicon-Labs/CP2102N-A02-GQFN20?qs=u16ybLDytRaG8WdlP0fT2g%3D%3D</t>
   </si>
   <si>
-    <t>Digi pote</t>
-  </si>
-  <si>
     <t>Bat to USB-c</t>
   </si>
   <si>
@@ -152,7 +137,55 @@
     <t>https://www.aliexpress.com/item/33016782798.html</t>
   </si>
   <si>
-    <t>https://www.mouser.ee/ProductDetail/Microchip-Technology-Atmel/MCP4019T-502E-LT?qs=%2FsslhGPpiOTvaIZO0TEW6Q%3D%3D</t>
+    <t>MOSFET 22A</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Nexperia/BUK6D22-30EX?qs=unwgFEO1A6ugfa8OC3vCnQ%3D%3D</t>
+  </si>
+  <si>
+    <t>Op amp</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Texas-Instruments/LM358DR?qs=Zu35EjizYSSY6pJ37yjmHA%3D%3D</t>
+  </si>
+  <si>
+    <t>display schottky</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/manufacturer/toshiba-semiconductors/</t>
+  </si>
+  <si>
+    <t>nmos 5A</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Panjit/PJA3404_R1_00001?qs=sPbYRqrBIVkiUO9ZInE3tw%3D%3D</t>
+  </si>
+  <si>
+    <t>Audio connector</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/CUI-Devices/SJ-3554A-SMT-TR-67?qs=l7cgNqFNU1hER9nK1Mk0ng%3D%3D</t>
+  </si>
+  <si>
+    <t>Audio DAC</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Texas-Instruments/PCM5100APWR?qs=E2%2FxqS9xjzplp26RZOMMKQ%3D%3D</t>
+  </si>
+  <si>
+    <t>3v3 power max</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/AATC/AS-1204B-LF?qs=uwxL4vQweFPVV%2FkgmXOg0A%3D%3D</t>
+  </si>
+  <si>
+    <t>Bat to 5V</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Monolithic-Power-Systems-MPS/MP28167GQ-P?qs=rkhjVJ6%2F3ELVPW%252BYAFTiog%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -202,8 +235,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hüperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normaallaad" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -219,7 +252,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office'i kujundus">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -481,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +526,7 @@
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -501,22 +534,29 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1">
         <f>SUM(E:E)</f>
-        <v>66.303200000000004</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>77.023200000000017</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1">
+        <f>SUM(I:I)</f>
+        <v>0.82471700000000014</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>1.43</v>
@@ -529,12 +569,12 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>14.15</v>
@@ -543,16 +583,19 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E28" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E44" si="0">C3*D3</f>
         <v>14.15</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>1.89</v>
@@ -564,8 +607,11 @@
         <f t="shared" si="0"/>
         <v>1.89</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>7.7000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -582,8 +628,11 @@
         <f t="shared" si="0"/>
         <v>10.98</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>2.9399999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -600,13 +649,16 @@
         <f t="shared" si="0"/>
         <v>4.3099999999999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
       </c>
       <c r="C7">
         <v>4.82</v>
@@ -618,8 +670,11 @@
         <f t="shared" si="0"/>
         <v>4.82</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -637,30 +692,12 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>36.909999999999997</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
       </c>
       <c r="C10">
         <v>3.79</v>
@@ -673,12 +710,12 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C11">
         <v>2.5499999999999998</v>
@@ -691,33 +728,42 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13">
+        <v>0.64</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.64</v>
+      </c>
+      <c r="I13">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>0.59</v>
@@ -729,13 +775,16 @@
         <f t="shared" si="0"/>
         <v>0.59</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C15">
         <f>9.86/100</f>
@@ -749,24 +798,24 @@
         <v>1.1831999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>2.16</v>
@@ -778,13 +827,16 @@
         <f t="shared" si="0"/>
         <v>2.16</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>1.37E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>6.64</v>
@@ -796,37 +848,52 @@
         <f t="shared" si="0"/>
         <v>6.64</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20">
+        <v>0.43</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C21">
-        <v>0.69</v>
+        <v>3.18</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>1.38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C22">
         <v>2.84</v>
@@ -839,12 +906,12 @@
         <v>5.68</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>0.96</v>
@@ -857,38 +924,197 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24">
+        <v>0.37</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26">
+        <v>3.45</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27">
+        <v>2.84</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E28">
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29">
+        <v>0.38</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1.1400000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30">
+        <v>0.37</v>
+      </c>
+      <c r="D30">
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
added adcin2 config description, fixed some rule check errors
</commit_message>
<xml_diff>
--- a/components.xlsx
+++ b/components.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>E-ink</t>
   </si>
@@ -83,9 +83,6 @@
     <t>https://www.aliexpress.com/item/1005004214252441.html</t>
   </si>
   <si>
-    <t>https://www.mouser.ee/ProductDetail/Texas-Instruments/TPS65988DJRSHR?qs=T3oQrply3y8cml9f5FMm3A%3D%3D</t>
-  </si>
-  <si>
     <t>USB-PD battery</t>
   </si>
   <si>
@@ -186,6 +183,15 @@
   </si>
   <si>
     <t>https://www.mouser.ee/ProductDetail/Monolithic-Power-Systems-MPS/MP28167GQ-P?qs=rkhjVJ6%2F3ELVPW%252BYAFTiog%3D%3D</t>
+  </si>
+  <si>
+    <t>parrallel to serial</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Texas-Instruments/SN74HCS16507PWR?qs=DPoM0jnrROUIT0uZVZ3kvw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Texas-Instruments/TPS65988DKRSHR?qs=DPoM0jnrROUevQj%2FLwa4Vw%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -517,7 +523,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,17 +540,17 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1">
         <f>SUM(E:E)</f>
-        <v>77.023200000000017</v>
+        <v>77.453199999999995</v>
       </c>
       <c r="I1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J1">
         <f>SUM(I:I)</f>
@@ -655,10 +661,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>4.82</v>
@@ -694,7 +700,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -715,7 +721,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11">
         <v>2.5499999999999998</v>
@@ -728,7 +734,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -739,10 +745,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
         <v>50</v>
-      </c>
-      <c r="B13" t="s">
-        <v>51</v>
       </c>
       <c r="C13">
         <v>0.64</v>
@@ -781,10 +787,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
       </c>
       <c r="C15">
         <f>9.86/100</f>
@@ -805,17 +811,29 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17">
+        <v>0.43</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
         <v>22</v>
-      </c>
-      <c r="B18" t="s">
-        <v>23</v>
       </c>
       <c r="C18">
         <v>2.16</v>
@@ -833,10 +851,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C19">
         <v>6.64</v>
@@ -854,10 +872,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
         <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
       </c>
       <c r="C20">
         <v>0.43</v>
@@ -872,10 +890,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
         <v>52</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
       </c>
       <c r="C21">
         <v>3.18</v>
@@ -890,10 +908,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
         <v>24</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
       </c>
       <c r="C22">
         <v>2.84</v>
@@ -908,10 +926,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
         <v>28</v>
-      </c>
-      <c r="B23" t="s">
-        <v>29</v>
       </c>
       <c r="C23">
         <v>0.96</v>
@@ -926,10 +944,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
         <v>39</v>
-      </c>
-      <c r="B24" t="s">
-        <v>40</v>
       </c>
       <c r="C24">
         <v>0.37</v>
@@ -944,10 +962,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
         <v>35</v>
-      </c>
-      <c r="B25" t="s">
-        <v>36</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
@@ -956,10 +974,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
         <v>45</v>
-      </c>
-      <c r="B26" t="s">
-        <v>46</v>
       </c>
       <c r="C26">
         <v>3.45</v>
@@ -974,10 +992,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
         <v>47</v>
-      </c>
-      <c r="B27" t="s">
-        <v>48</v>
       </c>
       <c r="C27">
         <v>2.84</v>
@@ -1001,10 +1019,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" t="s">
         <v>41</v>
-      </c>
-      <c r="B29" t="s">
-        <v>42</v>
       </c>
       <c r="C29">
         <v>0.38</v>
@@ -1019,10 +1037,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s">
         <v>43</v>
-      </c>
-      <c r="B30" t="s">
-        <v>44</v>
       </c>
       <c r="C30">
         <v>0.37</v>

</xml_diff>

<commit_message>
added nfc antenna components, added most of footprints
</commit_message>
<xml_diff>
--- a/components.xlsx
+++ b/components.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="25035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="10650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>E-ink</t>
   </si>
@@ -149,9 +149,6 @@
     <t>display schottky</t>
   </si>
   <si>
-    <t>https://www.mouser.ee/manufacturer/toshiba-semiconductors/</t>
-  </si>
-  <si>
     <t>nmos 5A</t>
   </si>
   <si>
@@ -192,6 +189,33 @@
   </si>
   <si>
     <t>https://www.mouser.ee/ProductDetail/Texas-Instruments/TPS65988DKRSHR?qs=DPoM0jnrROUevQj%2FLwa4Vw%3D%3D</t>
+  </si>
+  <si>
+    <t>JST XH 3p</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005003559631954.html</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/GCT/FFC2B35-24-T?qs=Li%252BoUPsLEnvLbIbV0OhDVA%3D%3D</t>
+  </si>
+  <si>
+    <t>FPC display conn</t>
+  </si>
+  <si>
+    <t>serial to parralel</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Nexperia/74HC595PW-Q100118?qs=1sbE9T7hb3aHrTORCcEuDg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Toshiba/CUHS20S30H3F?qs=PqoDHHvF64%252BnIC9Qnnw9zg%3D%3D</t>
+  </si>
+  <si>
+    <t>Resistor 5mO</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Vishay/WFCP06125L000FE66?qs=sGAEpiMZZMtlubZbdhIBIJBDgjsVQBFlUYEtiJor9t8%3D</t>
   </si>
 </sst>
 </file>
@@ -522,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,10 +571,10 @@
       </c>
       <c r="G1">
         <f>SUM(E:E)</f>
-        <v>77.453199999999995</v>
+        <v>78.933199999999999</v>
       </c>
       <c r="I1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J1">
         <f>SUM(I:I)</f>
@@ -698,6 +722,24 @@
         <v>1.24</v>
       </c>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9">
+        <v>0.47</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+    </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
@@ -745,10 +787,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
         <v>49</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
       </c>
       <c r="C13">
         <v>0.64</v>
@@ -805,17 +847,29 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16">
+        <v>0.43</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
         <v>53</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
       </c>
       <c r="C17">
         <v>0.43</v>
@@ -854,7 +908,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19">
         <v>6.64</v>
@@ -890,10 +944,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
         <v>51</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
       </c>
       <c r="C21">
         <v>3.18</v>
@@ -974,10 +1028,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
         <v>44</v>
-      </c>
-      <c r="B26" t="s">
-        <v>45</v>
       </c>
       <c r="C26">
         <v>3.45</v>
@@ -992,10 +1046,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
         <v>46</v>
-      </c>
-      <c r="B27" t="s">
-        <v>47</v>
       </c>
       <c r="C27">
         <v>2.84</v>
@@ -1022,7 +1076,7 @@
         <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C29">
         <v>0.38</v>
@@ -1037,10 +1091,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
         <v>42</v>
-      </c>
-      <c r="B30" t="s">
-        <v>43</v>
       </c>
       <c r="C30">
         <v>0.37</v>
@@ -1060,78 +1114,96 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
       <c r="E32">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
       <c r="E34">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E44">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
added inductors to component list
</commit_message>
<xml_diff>
--- a/components.xlsx
+++ b/components.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Tartu Ülikool - arvutitehnika\Riistvara projekt\airsoft_controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jako\Riistvara-projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>E-ink</t>
   </si>
@@ -216,6 +216,24 @@
   </si>
   <si>
     <t>https://www.mouser.ee/ProductDetail/Vishay/WFCP06125L000FE66?qs=sGAEpiMZZMtlubZbdhIBIJBDgjsVQBFlUYEtiJor9t8%3D</t>
+  </si>
+  <si>
+    <t>Inductor Bat cntr</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Bourns/SRP1265C-4R7M?qs=OlC7AqGiEDkg4Xkb2TDlFw%3D%3D</t>
+  </si>
+  <si>
+    <t>Inductor 5V</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Walsin/WLPMA0A040M4R7LC?qs=B6kkDfuK7%2FAGhXqtZ1HOFg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ee/ProductDetail/Taiyo-Yuden/NRS8030T1R0NJGJ?qs=PzICbMaShUfBDq1Kfb1D%252Bg%3D%3D</t>
+  </si>
+  <si>
+    <t>Inductor USB source</t>
   </si>
 </sst>
 </file>
@@ -265,8 +283,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hüperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normaallaad" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -282,7 +300,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office'i kujundus">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -546,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +589,7 @@
       </c>
       <c r="G1">
         <f>SUM(E:E)</f>
-        <v>78.933199999999999</v>
+        <v>81.923199999999994</v>
       </c>
       <c r="I1" t="s">
         <v>47</v>
@@ -1150,21 +1168,57 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35">
+        <v>1.5</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
       <c r="E35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36">
+        <v>0.67</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
       <c r="E36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37">
+        <v>0.41</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
       <c r="E37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>